<commit_message>
finished edges, started gameboard
</commit_message>
<xml_diff>
--- a/adjacentRules.xlsx
+++ b/adjacentRules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\92148\GithubProjects\SettlersOfCatan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\Desktop\Projet1.4\SettlersOfCatan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6F3E819-DDDA-4DB3-8436-6B7C3B6AA5F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EFF7FD-5B81-4AB9-8D3A-0AE3EDD70B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46764" yWindow="120" windowWidth="16176" windowHeight="12516" xr2:uid="{FF03602B-6CBE-4EDF-AA70-C15BD3C3834A}"/>
+    <workbookView xWindow="26730" yWindow="0" windowWidth="11775" windowHeight="20985" xr2:uid="{FF03602B-6CBE-4EDF-AA70-C15BD3C3834A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="40">
   <si>
     <t>0, 0, 0</t>
   </si>
@@ -90,6 +90,72 @@
   </si>
   <si>
     <t>vertice</t>
+  </si>
+  <si>
+    <t>resource</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>desert</t>
+  </si>
+  <si>
+    <t>wheat</t>
+  </si>
+  <si>
+    <t>whool</t>
+  </si>
+  <si>
+    <t>clay</t>
+  </si>
+  <si>
+    <t>ore</t>
+  </si>
+  <si>
+    <t>wood</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>L = q*2+1</t>
+  </si>
+  <si>
+    <t>2*(L-1) for r time</t>
+  </si>
+  <si>
+    <t>q axis</t>
+  </si>
+  <si>
+    <t>r pos</t>
+  </si>
+  <si>
+    <t>r neg</t>
+  </si>
+  <si>
+    <t>r axis</t>
+  </si>
+  <si>
+    <t>s pos</t>
+  </si>
+  <si>
+    <t>s neg</t>
+  </si>
+  <si>
+    <t>s axis</t>
+  </si>
+  <si>
+    <t>q pos</t>
+  </si>
+  <si>
+    <t>q neg</t>
   </si>
 </sst>
 </file>
@@ -444,25 +510,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8BBA882-6C62-484D-9B19-A0FA6EEF794D}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -473,7 +539,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -484,7 +550,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -495,7 +561,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -506,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -517,7 +583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -528,7 +594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0</v>
       </c>
@@ -539,7 +605,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C11">
         <v>0</v>
       </c>
@@ -565,7 +631,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>7</v>
       </c>
@@ -576,7 +642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -608,7 +674,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J14" s="1">
         <v>2</v>
       </c>
@@ -616,7 +682,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J15" s="1">
         <v>3</v>
       </c>
@@ -624,7 +690,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J16" s="1">
         <v>4</v>
       </c>
@@ -632,7 +698,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="10:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J17" s="1">
         <v>5</v>
       </c>
@@ -640,7 +706,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="10:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>17</v>
       </c>
@@ -654,7 +720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="10:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J20" s="1">
         <v>0</v>
       </c>
@@ -668,7 +734,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="10:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
+        <v>25</v>
+      </c>
       <c r="J21" s="1">
         <v>1</v>
       </c>
@@ -682,7 +769,28 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="10:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>4</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>3</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
       <c r="J22" s="1">
         <v>2</v>
       </c>
@@ -696,7 +804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="10:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J23" s="1">
         <v>3</v>
       </c>
@@ -710,7 +818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="10:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J24" s="1">
         <v>4</v>
       </c>
@@ -724,7 +832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="10:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J25" s="1">
         <v>5</v>
       </c>
@@ -736,6 +844,112 @@
       </c>
       <c r="M25">
         <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>31</v>
+      </c>
+      <c r="G29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>-2</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39">
+        <v>-3</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40">
+        <v>2</v>
+      </c>
+      <c r="C40">
+        <v>-3</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>